<commit_message>
fix : edit and delete data
</commit_message>
<xml_diff>
--- a/template excel uploaad/upload excel 2.xlsx
+++ b/template excel uploaad/upload excel 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\SiJak-21-LLDikti-III\template excel uploaad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\UNINDRAKu\magang\MSIB Batch 5\LLDIKTI III\Aplikasi Pajak SiJak\SiJak-21-LLDikti-III-main\template excel uploaad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3756D8B4-9AEB-43F7-A680-07A5290FFF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5383AF7E-E1C6-4753-B664-8C6EFCF26C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19905" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upload excel" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>no_H01</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>Himsar Silaban</t>
+  </si>
+  <si>
+    <t>pembatalan_H03</t>
+  </si>
+  <si>
+    <t>195303071975081000</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -680,10 +689,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1039,54 +1051,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="41.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="21.1796875" customWidth="1"/>
-    <col min="38" max="38" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="21.140625" customWidth="1"/>
+    <col min="39" max="39" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1094,448 +1107,457 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2000000003</v>
       </c>
       <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>45020</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>98098</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="3">
         <v>1230912</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>45292</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>1234570000000000</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1000000</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>300000</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>15000</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1035150</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>240000</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>123132</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>1000</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>120031</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>1312218</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>131230</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>13913129</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>109310391</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>121320</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>132412</v>
-      </c>
-      <c r="AC2">
-        <v>123123</v>
       </c>
       <c r="AD2">
         <v>123123</v>
       </c>
       <c r="AE2">
+        <v>123123</v>
+      </c>
+      <c r="AF2">
         <v>12391</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>1023910</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>123123</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>131321</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>0</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>21</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>12</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000000002</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>45020</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>321321</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="3">
         <v>1230912</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>45292</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>1234570000000000</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1000000</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>300000</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>15000</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>1035150</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>240000</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>123132</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>1000</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>120031</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>1312218</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>0</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>131230</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>13913129</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>109310391</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>121320</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>132412</v>
-      </c>
-      <c r="AC3">
-        <v>123123</v>
       </c>
       <c r="AD3">
         <v>123123</v>
       </c>
       <c r="AE3">
+        <v>123123</v>
+      </c>
+      <c r="AF3">
         <v>12391</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>1023910</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>123123</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>131321</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>0</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>21</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>12</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000000001</v>
       </c>
       <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>45017</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>688861822432000</v>
       </c>
-      <c r="E4" s="2">
-        <v>1.9530307197508099E+17</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>32649</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>37</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>1234570000000000</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>22646899</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>2264680</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>24911579</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>5400147</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>579360</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>30891086</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>691667</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>31582753</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>1579133</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>1494133</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>3073266</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>28509487</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>85528461</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>27028000</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>450466</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>223345</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>450466</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -1543,7 +1565,129 @@
       <c r="AK4">
         <v>0</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000000002</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45386</v>
+      </c>
+      <c r="E5" s="2">
+        <v>321321</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1230912</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45292</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1234570000000000</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5">
+        <v>1000000</v>
+      </c>
+      <c r="P5">
+        <v>300000</v>
+      </c>
+      <c r="Q5">
+        <v>15000</v>
+      </c>
+      <c r="R5">
+        <v>1035150</v>
+      </c>
+      <c r="S5">
+        <v>240000</v>
+      </c>
+      <c r="T5">
+        <v>123132</v>
+      </c>
+      <c r="U5">
+        <v>1000</v>
+      </c>
+      <c r="V5">
+        <v>120031</v>
+      </c>
+      <c r="W5">
+        <v>1312218</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>131230</v>
+      </c>
+      <c r="Z5">
+        <v>13913129</v>
+      </c>
+      <c r="AA5">
+        <v>109310391</v>
+      </c>
+      <c r="AB5">
+        <v>121320</v>
+      </c>
+      <c r="AC5">
+        <v>132412</v>
+      </c>
+      <c r="AD5">
+        <v>123123</v>
+      </c>
+      <c r="AE5">
+        <v>123123</v>
+      </c>
+      <c r="AF5">
+        <v>12391</v>
+      </c>
+      <c r="AG5">
+        <v>1023910</v>
+      </c>
+      <c r="AH5">
+        <v>123123</v>
+      </c>
+      <c r="AI5">
+        <v>131321</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK5">
+        <v>21</v>
+      </c>
+      <c r="AL5">
+        <v>12</v>
+      </c>
+      <c r="AM5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>